<commit_message>
Update Climate Weather Properties.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Climate Weather Properties.xlsx
+++ b/Documents/Climate Weather Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC06260-88D7-44D9-B075-34C1532FCFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66336822-9F70-4562-A843-D344B16A5922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>Weather Features</t>
   </si>
@@ -194,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -610,15 +610,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -650,6 +641,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,58 +695,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -819,52 +831,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -1173,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,71 +1150,71 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="16"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="50"/>
     </row>
     <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12" t="s">
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="12" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="12" t="s">
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="12" t="s">
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="13"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -1328,262 +1294,314 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="55"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="56"/>
     </row>
     <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23" t="s">
+      <c r="F5" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="27" t="s">
+      <c r="M5" s="18"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="23"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="25"/>
+      <c r="S5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" s="20"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="19"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="34" t="s">
+      <c r="F6" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="30"/>
+      <c r="W6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="36"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="32" t="s">
+      <c r="G7" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="36"/>
+      <c r="J7" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="27"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="30"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="29"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="42" t="s">
+      <c r="F8" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="45" t="s">
+      <c r="J8" s="33"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="34"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="45" t="s">
+      <c r="T8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="V8" s="32"/>
+      <c r="W8" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="36"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="29"/>
     </row>
     <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="47" t="s">
+      <c r="C9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="47" t="s">
+      <c r="E9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="49" t="s">
+      <c r="G9" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="49"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="48"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="39"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="T9" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="V9" s="38"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1595,26 +1613,26 @@
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",F11)))</formula>
+  <conditionalFormatting sqref="B5:Y9">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Moderate-High">
+      <formula>NOT(ISERROR(SEARCH("Moderate-High",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Moderate-Low">
+      <formula>NOT(ISERROR(SEARCH("Moderate-Low",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:Y9">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Moderate-High">
-      <formula>NOT(ISERROR(SEARCH("Moderate-High",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Moderate-Low">
-      <formula>NOT(ISERROR(SEARCH("Moderate-Low",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",B5)))</formula>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data tables, finished spreadsheet, basic niagara
</commit_message>
<xml_diff>
--- a/Documents/Climate Weather Properties.xlsx
+++ b/Documents/Climate Weather Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C Documents\GitHub\ToolsDevForEngines\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66336822-9F70-4562-A843-D344B16A5922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF597BF-4E55-46DE-BFD9-83690535F4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="23">
   <si>
     <t>Weather Features</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Winter</t>
   </si>
   <si>
-    <t>Sun</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>Moderate-High</t>
+  </si>
+  <si>
+    <t>Cloud Coverage</t>
+  </si>
+  <si>
+    <t>Moderate-lOw</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -641,8 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -652,29 +653,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,15 +698,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,84 +1145,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="50"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="46"/>
     </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="46" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="46" t="s">
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="46" t="s">
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="46" t="s">
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="47"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="43"/>
     </row>
-    <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1293,317 +1300,422 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="44"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="56"/>
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="41"/>
     </row>
-    <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="X5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="W7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y7" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="52" t="s">
+      <c r="B9" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="V9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="W9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="X9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" s="20"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="19"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="30"/>
-      <c r="W6" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="29"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="27"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="T7" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="U7" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="V7" s="30"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="29"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="T8" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="V8" s="32"/>
-      <c r="W8" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="29"/>
-    </row>
-    <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="39"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="39"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="S9" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="V9" s="38"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="40"/>
+      <c r="Y9" s="33" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M9">
+    <sortCondition ref="A5:A9"/>
+  </sortState>
   <mergeCells count="7">
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="B1:Y1"/>

</xml_diff>

<commit_message>
fixed day length i think. however i now NEED to fix the issue of the brush for the volume not showing up in editor.
</commit_message>
<xml_diff>
--- a/Documents/Climate Weather Properties.xlsx
+++ b/Documents/Climate Weather Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ACC73F-5497-4D6B-B9D1-8F677F15860C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CADDB3-C184-4167-BA30-484E23324CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5676" yWindow="528" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1146,16 +1146,16 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="56" t="s">
         <v>0</v>
@@ -1184,7 +1184,7 @@
       <c r="X1" s="57"/>
       <c r="Y1" s="58"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="59" t="s">
         <v>2</v>
@@ -1223,7 +1223,7 @@
       <c r="X2" s="54"/>
       <c r="Y2" s="55"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36"/>
       <c r="B4" s="40"/>
       <c r="C4" s="37"/>
@@ -1327,7 +1327,7 @@
       <c r="X4" s="37"/>
       <c r="Y4" s="41"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="47" t="s">
         <v>19</v>
@@ -1404,7 +1404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
fixed crash if no season or climate selected. made day night box look better. day night is now false by default. filled in data table. cleaned up my euw code quite a bit. also wrote forum posts! next big focus is calculations
</commit_message>
<xml_diff>
--- a/Documents/Climate Weather Properties.xlsx
+++ b/Documents/Climate Weather Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C Documents\GitHub\ToolsDevForEngines\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CADDB3-C184-4167-BA30-484E23324CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9D6B6B-58AF-45CA-B97F-8B68758774C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="528" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1146,16 +1146,16 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="56" t="s">
         <v>0</v>
@@ -1184,7 +1184,7 @@
       <c r="X1" s="57"/>
       <c r="Y1" s="58"/>
     </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="59" t="s">
         <v>2</v>
@@ -1223,7 +1223,7 @@
       <c r="X2" s="54"/>
       <c r="Y2" s="55"/>
     </row>
-    <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36"/>
       <c r="B4" s="40"/>
       <c r="C4" s="37"/>
@@ -1327,7 +1327,7 @@
       <c r="X4" s="37"/>
       <c r="Y4" s="41"/>
     </row>
-    <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>19</v>
@@ -1558,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
commented code. still need to update wind values
</commit_message>
<xml_diff>
--- a/Documents/Climate Weather Properties.xlsx
+++ b/Documents/Climate Weather Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9D6B6B-58AF-45CA-B97F-8B68758774C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE08D82-2D8A-4AD4-B155-B481D8A27AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="22">
   <si>
     <t>Weather Features</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Wind</t>
-  </si>
-  <si>
-    <t>Fog</t>
   </si>
   <si>
     <t>Thunder</t>
@@ -623,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -710,6 +707,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,7 +1145,7 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,10 +1155,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="56" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="57"/>
       <c r="C1" s="57"/>
       <c r="D1" s="57"/>
       <c r="E1" s="57"/>
@@ -1178,11 +1177,11 @@
       <c r="R1" s="57"/>
       <c r="S1" s="57"/>
       <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="61"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
@@ -1211,93 +1210,75 @@
       <c r="P2" s="54"/>
       <c r="Q2" s="55"/>
       <c r="R2" s="54" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="S2" s="54"/>
       <c r="T2" s="54"/>
       <c r="U2" s="55"/>
-      <c r="V2" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="55"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="N3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="R3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1321,293 +1302,253 @@
       <c r="R4" s="37"/>
       <c r="S4" s="37"/>
       <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="41"/>
+      <c r="U4" s="41"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="F5" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="K5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="Q5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>16</v>
-      </c>
       <c r="R5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="19" t="s">
-        <v>16</v>
+      <c r="S5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="X5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y5" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="K6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="22" t="s">
+      <c r="M6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="23" t="s">
+      <c r="N6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>18</v>
-      </c>
       <c r="P6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="24" t="s">
         <v>19</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="V6" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="W6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y6" s="24" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="22" t="s">
+      <c r="K7" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="M7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="P7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="R7" s="25" t="s">
-        <v>18</v>
-      </c>
       <c r="S7" s="23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="T7" s="23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="U7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="V7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="W7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="X7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="J8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>19</v>
-      </c>
       <c r="L8" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="R8" s="26" t="s">
@@ -1620,112 +1561,87 @@
         <v>19</v>
       </c>
       <c r="U8" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="V8" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="W8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="X8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="O9" s="34" t="s">
         <v>16</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q9" s="33" t="s">
         <v>17</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S9" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="T9" s="34" t="s">
         <v>18</v>
       </c>
       <c r="U9" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="V9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="W9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="X9" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y9" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M9">
     <sortCondition ref="A5:A9"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:Y1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="R2:U2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:Y9">
+  <conditionalFormatting sqref="B5:U9">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Moderate-High">
       <formula>NOT(ISERROR(SEARCH("Moderate-High",B5)))</formula>
     </cfRule>

</xml_diff>